<commit_message>
Updated scedule and charter
</commit_message>
<xml_diff>
--- a/Documentation/Project Plan 13th of October to 8th of December.xlsx
+++ b/Documentation/Project Plan 13th of October to 8th of December.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="45">
   <si>
     <t>Week 1 13-10-2015</t>
   </si>
@@ -146,6 +146,9 @@
   </si>
   <si>
     <t xml:space="preserve">Continue work on coding </t>
+  </si>
+  <si>
+    <t>Fill in project charter</t>
   </si>
 </sst>
 </file>
@@ -556,8 +559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -743,7 +746,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>